<commit_message>
fix: remove leading and trailing spaces in address fields instead of using normalize-space function in the XSLT file for HL7 #2739 - updated Patient address, relationship address and Organization address. - remove "urn:oid:" if already present in the system value for race and ethnicity of patient resource. - updated mapping document
</commit_message>
<xml_diff>
--- a/support/specifications/hl7/HL7v2.to.FHIR.Conversion.Spec.xlsx
+++ b/support/specifications/hl7/HL7v2.to.FHIR.Conversion.Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="9"/>
+    <workbookView windowWidth="19200" windowHeight="8000" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="435">
   <si>
     <t>FHIR Resources</t>
   </si>
@@ -201,6 +201,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Uses the </t>
     </r>
     <r>
@@ -1702,6 +1709,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">The OBX segment in which </t>
     </r>
     <r>
@@ -3026,6 +3039,9 @@
     <t>"http://shinny.org/us/ny/hrsn/Encounter/&lt;encounterResourceId&gt;"</t>
   </si>
   <si>
+    <t>Remark</t>
+  </si>
+  <si>
     <t>"Organization"</t>
   </si>
   <si>
@@ -3039,6 +3055,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Provided the fixed value as "true". 
 </t>
     </r>
@@ -3061,6 +3083,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"identifier" : [{
         "type" : {
           "coding" : [{
@@ -3118,6 +3147,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Mapped from the header variable '</t>
     </r>
     <r>
@@ -3139,7 +3175,17 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>'</t>
+      <t xml:space="preserve">'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Both TAX and NPI numbers will be added to the Identifier if available.</t>
     </r>
   </si>
   <si>
@@ -3171,6 +3217,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"identifier" : [{
         "type" : {
           "coding" : [{
@@ -3228,6 +3281,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Mapped from the header variable, </t>
     </r>
     <r>
@@ -3249,7 +3309,17 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.</t>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Both TAX and NPI numbers will be added to the Identifier if available.</t>
     </r>
   </si>
   <si>
@@ -3284,6 +3354,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Mapped from the header variable,  </t>
     </r>
     <r>
@@ -3303,6 +3380,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"type" : [{
         "coding" : [{
           "system" : "http://terminology.hl7.org/CodeSystem/organization-type",
@@ -3350,6 +3434,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"telecom" : [{
       "system" : "phone",
       "</t>
@@ -3473,11 +3564,39 @@
     <t>ORC.23.2</t>
   </si>
   <si>
-    <t>WP'  - &gt; work
-'H'  - &gt; home
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WP'  - &gt; work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'H'  - &gt; home</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 'TMP'  - &gt; temp
 'MC' or 'PG' - &gt; mobile
 Otherwise -&gt; ORC.23.2</t>
+    </r>
   </si>
   <si>
     <t>ORC.22.1 + OR.C22.2 + ORC.22.3 + ORC.22.4 + ORC.22.5 + ORC.22.6</t>
@@ -3500,11 +3619,39 @@
     <t>ORC.22.7</t>
   </si>
   <si>
-    <t>WP'  - &gt; work
-'H' or 'HP' - &gt; home
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WP'  - &gt; work
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'H' or 'HP' - &gt; home</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 'TMP'  - &gt; temp
 'OLD' or 'BAD' - &gt; old
 Otherwise -&gt; ORC.22.7</t>
+    </r>
   </si>
   <si>
     <t>ORC22.1 + ORC22.2 (note: ORC22.1 and ORC22.2 have different meanings for a company address than for a person address)</t>
@@ -4209,6 +4356,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>If the screening code is one of ('</t>
     </r>
     <r>
@@ -4966,11 +5119,25 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -4983,16 +5150,10 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -5010,17 +5171,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="40">
@@ -5548,7 +5701,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5579,9 +5732,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -5636,21 +5786,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5669,30 +5804,18 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5708,12 +5831,12 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5735,38 +5858,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5865,7 +5970,7 @@
     <cellStyle name="Warning" xfId="59"/>
   </cellStyles>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{10E1960B-19B8-46C3-8A96-6E0ED43A31EE}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{79655ED8-46CF-41F3-B049-9A522ABE8835}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6139,80 +6244,80 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8571428571429" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11.8545454545455" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="14.2857142857143" style="80" customWidth="1"/>
+    <col min="1" max="1" width="14.2818181818182" style="64" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="123.571428571429" customWidth="1"/>
+    <col min="3" max="3" width="123.572727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
-      <c r="B2" s="19"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76" t="s">
+      <c r="A8" s="60"/>
+      <c r="B8" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="53" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76" t="s">
+      <c r="A9" s="60"/>
+      <c r="B9" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="53" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76" t="s">
+      <c r="A10" s="60"/>
+      <c r="B10" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="53" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" ht="45" spans="1:3">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76" t="s">
+    <row r="11" ht="43.5" spans="1:3">
+      <c r="A11" s="60"/>
+      <c r="B11" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="63" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="76"/>
-      <c r="B12" s="79" t="s">
+      <c r="A12" s="60"/>
+      <c r="B12" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="76"/>
-      <c r="B13" s="76" t="s">
+      <c r="A13" s="60"/>
+      <c r="B13" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="76"/>
-      <c r="B14" s="76"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1.39370078740157" bottom="1.39370078740157" header="1" footer="1"/>
@@ -6226,21 +6331,21 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.5714285714286" style="2" customWidth="1"/>
-    <col min="3" max="3" width="49.6666666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.552380952381" style="2" customWidth="1"/>
-    <col min="5" max="5" width="53.2857142857143" style="2" customWidth="1"/>
-    <col min="6" max="6" width="47.5714285714286" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.14285714285714" style="2"/>
+    <col min="1" max="1" width="14.7181818181818" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.5727272727273" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.6636363636364" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.5545454545455" style="2" customWidth="1"/>
+    <col min="5" max="5" width="53.2818181818182" style="2" customWidth="1"/>
+    <col min="6" max="6" width="47.5727272727273" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.14545454545454" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6251,16 +6356,16 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="17" customHeight="1" spans="1:6">
@@ -6279,7 +6384,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
@@ -6291,7 +6396,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:6">
@@ -6306,12 +6411,12 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" s="2" customFormat="1" ht="30" spans="2:6">
+    <row r="6" s="2" customFormat="1" ht="29" spans="2:6">
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -6326,149 +6431,149 @@
         <v>43</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="1" ht="150" spans="2:5">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="145" spans="2:5">
       <c r="B8" s="6" t="s">
         <v>179</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="409" customHeight="1" spans="2:5">
       <c r="B9" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="10" t="s">
-        <v>418</v>
+      <c r="D9" s="5" t="s">
+        <v>419</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="1" ht="150" spans="2:5">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" ht="145" spans="2:5">
       <c r="B10" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="D10" s="10" t="s">
         <v>421</v>
       </c>
+      <c r="D10" s="5" t="s">
+        <v>422</v>
+      </c>
       <c r="E10" s="8" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="180" spans="2:5">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="159.5" spans="2:5">
       <c r="B11" s="6" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="2"/>
       <c r="E11" s="9" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="12" s="2" customFormat="1" ht="150" spans="2:5">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1" ht="145" spans="2:5">
       <c r="B12" s="6" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="2"/>
       <c r="E12" s="9" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="13" s="2" customFormat="1" ht="75" spans="2:4">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" ht="58" spans="2:4">
       <c r="B13" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="14" s="2" customFormat="1" ht="30" spans="2:3">
+      <c r="C13" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="29" spans="2:3">
       <c r="B14" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="15" s="2" customFormat="1" ht="45" spans="2:4">
+    <row r="15" s="2" customFormat="1" ht="43.5" spans="2:4">
       <c r="B15" s="6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="30" spans="2:5">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="29" spans="2:5">
       <c r="B16" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="E16" s="13" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="17" s="2" customFormat="1" ht="45" spans="2:4">
+      <c r="E16" s="12" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="1" ht="43.5" spans="2:4">
       <c r="B17" s="6" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" spans="2:6">
       <c r="B18" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="14" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="19" s="2" customFormat="1" ht="165" spans="2:5">
+      <c r="F18" s="13" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="19" s="2" customFormat="1" ht="159.5" spans="2:5">
       <c r="B19" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" spans="2:4">
@@ -6478,8 +6583,8 @@
       <c r="C20" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>433</v>
+      <c r="D20" s="14" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -6487,9 +6592,9 @@
         <v>173</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="D21" s="15"/>
+        <v>378</v>
+      </c>
+      <c r="D21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6512,96 +6617,96 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" style="76" customWidth="1"/>
-    <col min="2" max="2" width="28.2857142857143" style="76" customWidth="1"/>
-    <col min="3" max="3" width="66.4285714285714" style="76" customWidth="1"/>
-    <col min="4" max="4" width="46.2857142857143" style="76" customWidth="1"/>
+    <col min="1" max="1" width="14.7181818181818" style="60" customWidth="1"/>
+    <col min="2" max="2" width="28.2818181818182" style="60" customWidth="1"/>
+    <col min="3" max="3" width="66.4272727272727" style="60" customWidth="1"/>
+    <col min="4" max="4" width="46.2818181818182" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="61" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="62" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="78"/>
-      <c r="B3" s="76" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="60" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="78"/>
-      <c r="B4" s="76" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="60" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" ht="90" spans="2:4">
-      <c r="B5" s="76" t="s">
+    <row r="5" ht="87" spans="2:4">
+      <c r="B5" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="63" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="63"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="79"/>
+      <c r="D7" s="63"/>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" ht="30" spans="2:3">
-      <c r="B9" s="76" t="s">
+    <row r="9" ht="29" spans="2:3">
+      <c r="B9" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="63" t="s">
         <v>33</v>
       </c>
     </row>
@@ -6646,10 +6751,10 @@
       <c r="C21"/>
     </row>
     <row r="22" hidden="1" spans="2:3">
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6667,566 +6772,566 @@
   <sheetPr/>
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.1142857142857" customWidth="1"/>
-    <col min="2" max="2" width="39.1428571428571" style="12" customWidth="1"/>
-    <col min="3" max="3" width="61.5714285714286" style="12" customWidth="1"/>
-    <col min="4" max="4" width="66.8571428571429" style="12" customWidth="1"/>
-    <col min="5" max="5" width="64.5714285714286" style="12" customWidth="1"/>
-    <col min="6" max="256" width="11.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="13.1181818181818" customWidth="1"/>
+    <col min="2" max="2" width="39.1454545454545" style="11" customWidth="1"/>
+    <col min="3" max="3" width="61.5727272727273" style="11" customWidth="1"/>
+    <col min="4" max="4" width="66.8545454545455" style="11" customWidth="1"/>
+    <col min="5" max="5" width="64.5727272727273" style="11" customWidth="1"/>
+    <col min="6" max="256" width="11.8545454545455" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="1" spans="1:5">
-      <c r="A1" s="16" t="s">
+    <row r="1" s="17" customFormat="1" spans="1:5">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="24"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="24"/>
-    </row>
-    <row r="6" ht="30" spans="2:5">
-      <c r="B6" s="20" t="s">
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" ht="60" spans="2:5">
-      <c r="B7" s="12" t="s">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" ht="58" spans="2:5">
+      <c r="B7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" ht="60" spans="2:5">
-      <c r="B8" s="12" t="s">
+    <row r="8" ht="58" spans="2:5">
+      <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="24"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13" ht="60" spans="2:5">
-      <c r="B13" s="12" t="s">
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" ht="58" spans="2:5">
+      <c r="B13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="24"/>
-    </row>
-    <row r="14" ht="30" spans="2:5">
-      <c r="B14" s="12" t="s">
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" ht="29" spans="2:5">
+      <c r="B14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="24"/>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" ht="120" spans="2:5">
-      <c r="B17" s="12" t="s">
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" ht="116" spans="2:5">
+      <c r="B17" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="24"/>
-    </row>
-    <row r="18" ht="30" spans="2:5">
-      <c r="B18" s="12" t="s">
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" ht="29" spans="2:5">
+      <c r="B18" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="24"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="24"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="23"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="23"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="24"/>
-    </row>
-    <row r="25" ht="75" spans="2:5">
-      <c r="B25" s="12" t="s">
+      <c r="E24" s="23"/>
+    </row>
+    <row r="25" ht="72.5" spans="2:5">
+      <c r="B25" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="24"/>
-    </row>
-    <row r="26" ht="45" spans="2:5">
-      <c r="B26" s="28" t="s">
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" ht="29" spans="2:5">
+      <c r="B26" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="70" t="s">
+      <c r="C26" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" ht="30" spans="2:5">
-      <c r="B27" s="28" t="s">
+    <row r="27" ht="29" spans="2:5">
+      <c r="B27" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="70" t="s">
+      <c r="C27" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="71"/>
-      <c r="E27" s="73"/>
-    </row>
-    <row r="28" ht="30" spans="2:5">
-      <c r="B28" s="28" t="s">
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="73"/>
-    </row>
-    <row r="29" ht="30" spans="2:5">
-      <c r="B29" s="28" t="s">
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
+    </row>
+    <row r="29" ht="29" spans="2:5">
+      <c r="B29" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="71"/>
-      <c r="E29" s="73"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="57"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="71"/>
+      <c r="D30" s="56"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" ht="30" spans="2:5">
-      <c r="B31" s="28" t="s">
+    <row r="31" ht="29" spans="2:5">
+      <c r="B31" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="71" t="s">
+      <c r="D31" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="72" t="s">
+      <c r="E31" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" ht="30" spans="2:5">
-      <c r="B32" s="28" t="s">
+    <row r="32" ht="29" spans="2:5">
+      <c r="B32" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="71"/>
-      <c r="E32" s="73"/>
-    </row>
-    <row r="33" ht="30" spans="2:5">
-      <c r="B33" s="28" t="s">
+      <c r="D32" s="56"/>
+      <c r="E32" s="57"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="71"/>
-      <c r="E33" s="73"/>
-    </row>
-    <row r="34" ht="30" spans="2:5">
-      <c r="B34" s="28" t="s">
+      <c r="D33" s="56"/>
+      <c r="E33" s="57"/>
+    </row>
+    <row r="34" ht="29" spans="2:5">
+      <c r="B34" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="71"/>
-      <c r="E34" s="73"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="57"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="71"/>
-      <c r="E35" s="73"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="57"/>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="71" t="s">
+      <c r="D36" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="73"/>
-    </row>
-    <row r="37" ht="45" spans="2:5">
-      <c r="B37" s="28" t="s">
+      <c r="E36" s="57"/>
+    </row>
+    <row r="37" ht="43.5" spans="2:5">
+      <c r="B37" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="71"/>
-      <c r="E37" s="81" t="s">
+      <c r="D37" s="56"/>
+      <c r="E37" s="65" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="38" ht="135" spans="2:5">
-      <c r="B38" s="74" t="s">
+    <row r="38" ht="130.5" spans="2:5">
+      <c r="B38" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74" t="s">
+      <c r="C38" s="58"/>
+      <c r="D38" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="39" ht="135" spans="2:5">
-      <c r="B39" s="74" t="s">
+    <row r="39" ht="130.5" spans="2:5">
+      <c r="B39" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74" t="s">
+      <c r="C39" s="58"/>
+      <c r="D39" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="23" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="23"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="E41" s="24"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E42" s="24"/>
+      <c r="E42" s="23"/>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E43" s="24"/>
-    </row>
-    <row r="44" ht="195" spans="2:5">
-      <c r="B44" s="20" t="s">
+      <c r="E43" s="23"/>
+    </row>
+    <row r="44" ht="188.5" spans="2:5">
+      <c r="B44" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E44" s="24"/>
-    </row>
-    <row r="45" ht="195" spans="2:5">
-      <c r="B45" s="20" t="s">
+      <c r="E44" s="23"/>
+    </row>
+    <row r="45" ht="188.5" spans="2:5">
+      <c r="B45" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="64" t="s">
+      <c r="D45" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="57" t="s">
+      <c r="E45" s="47" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="46" ht="195" spans="2:5">
-      <c r="B46" s="20" t="s">
+    <row r="46" ht="188.5" spans="2:5">
+      <c r="B46" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E46" s="24"/>
+      <c r="E46" s="23"/>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E47" s="24"/>
+      <c r="E47" s="23"/>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="E48" s="24"/>
+      <c r="E48" s="23"/>
     </row>
     <row r="49" spans="2:5">
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E49" s="24"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E50" s="24"/>
-    </row>
-    <row r="51" ht="150" spans="2:5">
-      <c r="B51" s="12" t="s">
+      <c r="E50" s="23"/>
+    </row>
+    <row r="51" ht="145" spans="2:5">
+      <c r="B51" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="11" t="s">
         <v>142</v>
       </c>
       <c r="E51" s="8" t="s">
@@ -7234,149 +7339,149 @@
       </c>
     </row>
     <row r="52" spans="2:5">
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="E52" s="24"/>
+      <c r="E52" s="23"/>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E53" s="24"/>
+      <c r="E53" s="23"/>
     </row>
     <row r="54" spans="2:5">
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="E54" s="24"/>
+      <c r="E54" s="23"/>
     </row>
     <row r="55" spans="2:5">
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E55" s="24"/>
+      <c r="E55" s="23"/>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E56" s="24"/>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="2:5">
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C57" s="25" t="s">
+      <c r="C57" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="E57" s="24"/>
-    </row>
-    <row r="58" ht="180" spans="2:5">
-      <c r="B58" s="12" t="s">
+      <c r="E57" s="23"/>
+    </row>
+    <row r="58" ht="174" spans="2:5">
+      <c r="B58" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C58" s="25" t="s">
+      <c r="C58" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E58" s="24"/>
-    </row>
-    <row r="59" ht="90" spans="2:5">
-      <c r="B59" s="66" t="s">
+      <c r="E58" s="23"/>
+    </row>
+    <row r="59" ht="72.5" spans="2:5">
+      <c r="B59" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="C59" s="66"/>
-      <c r="D59" s="66" t="s">
+      <c r="C59" s="27"/>
+      <c r="D59" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="E59" s="24"/>
-    </row>
-    <row r="60" ht="255" spans="2:5">
-      <c r="B60" s="12" t="s">
+      <c r="E59" s="23"/>
+    </row>
+    <row r="60" ht="246.5" spans="2:5">
+      <c r="B60" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E60" s="24" t="s">
+      <c r="E60" s="23" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="61" ht="135" spans="2:5">
-      <c r="B61" s="12" t="s">
+    <row r="61" ht="130.5" spans="2:5">
+      <c r="B61" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E61" s="24"/>
-    </row>
-    <row r="62" ht="30" spans="2:5">
-      <c r="B62" s="12" t="s">
+      <c r="E61" s="23"/>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="E62" s="24"/>
+      <c r="E62" s="23"/>
     </row>
     <row r="63" spans="2:5">
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E63" s="24"/>
+      <c r="E63" s="23"/>
     </row>
     <row r="64" spans="2:5">
-      <c r="B64" s="12" t="s">
+      <c r="B64" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D64" s="75" t="s">
+      <c r="D64" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="E64" s="24"/>
+      <c r="E64" s="23"/>
     </row>
     <row r="65" ht="42.95" customHeight="1" spans="2:5">
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C65" s="69" t="s">
+      <c r="C65" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="D65" s="75"/>
-      <c r="E65" s="24"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="23"/>
     </row>
     <row r="68" spans="3:3">
-      <c r="C68" s="69"/>
+      <c r="C68" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7406,82 +7511,82 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" customWidth="1"/>
-    <col min="2" max="2" width="40.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="61.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="57.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="54.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
+    <col min="1" max="1" width="9.14545454545454" customWidth="1"/>
+    <col min="2" max="2" width="40.8545454545455" customWidth="1"/>
+    <col min="3" max="3" width="61.5727272727273" customWidth="1"/>
+    <col min="4" max="4" width="57.4272727272727" customWidth="1"/>
+    <col min="5" max="5" width="54.8545454545455" customWidth="1"/>
+    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="24"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>178</v>
       </c>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" ht="45" spans="2:5">
-      <c r="B7" s="19" t="s">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" ht="29" spans="2:5">
+      <c r="B7" s="18" t="s">
         <v>179</v>
       </c>
       <c r="C7" t="s">
@@ -7490,18 +7595,18 @@
       <c r="D7" t="s">
         <v>181</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="50" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" ht="135" spans="2:5">
-      <c r="B8" s="61" t="s">
+    <row r="8" ht="130.5" spans="2:5">
+      <c r="B8" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="52" t="s">
         <v>185</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -7509,43 +7614,43 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="24"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="24" t="s">
+      <c r="D10" s="26"/>
+      <c r="E10" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" ht="225" spans="2:5">
-      <c r="B11" s="19" t="s">
+    <row r="11" ht="217.5" spans="2:5">
+      <c r="B11" s="18" t="s">
         <v>192</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>195</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -7556,18 +7661,18 @@
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="2" t="s">
         <v>198</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="14" ht="30" spans="2:5">
-      <c r="B14" s="19" t="s">
+    <row r="14" ht="29" spans="2:5">
+      <c r="B14" s="18" t="s">
         <v>199</v>
       </c>
       <c r="C14" t="s">
@@ -7576,70 +7681,70 @@
       <c r="D14" t="s">
         <v>201</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="23" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="15" ht="45" spans="2:5">
-      <c r="B15" s="19" t="s">
+    <row r="15" ht="43.5" spans="2:5">
+      <c r="B15" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="50" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="16" ht="45" spans="2:5">
-      <c r="B16" s="19" t="s">
+    <row r="16" ht="43.5" spans="2:5">
+      <c r="B16" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" ht="60" spans="2:5">
-      <c r="B17" s="61" t="s">
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" ht="58" spans="2:5">
+      <c r="B17" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="D17" s="66" t="s">
+      <c r="D17" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="E17" s="24"/>
-    </row>
-    <row r="18" ht="60" spans="2:5">
-      <c r="B18" s="67" t="s">
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" ht="58" spans="2:5">
+      <c r="B18" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="19" ht="60" spans="2:5">
+    <row r="19" spans="2:5">
       <c r="B19" s="6" t="s">
         <v>216</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D19" s="66" t="s">
+      <c r="D19" s="27" t="s">
         <v>218</v>
       </c>
       <c r="E19" s="8" t="s">
@@ -7653,32 +7758,32 @@
       <c r="C20" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D20" s="66"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="8" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="21" ht="77" customHeight="1" spans="2:5">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="24"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="24"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7702,87 +7807,87 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" customWidth="1"/>
+    <col min="1" max="1" width="9.14545454545454" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="43.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="57.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
+    <col min="4" max="4" width="43.5727272727273" customWidth="1"/>
+    <col min="5" max="5" width="57.5727272727273" customWidth="1"/>
+    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="24"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="24"/>
-    </row>
-    <row r="6" ht="30" spans="2:5">
-      <c r="B6" s="20" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" ht="29" spans="2:5">
+      <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="11"/>
       <c r="D7" t="s">
         <v>226</v>
       </c>
@@ -7790,73 +7895,72 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" ht="75" spans="2:5">
-      <c r="B8" s="19" t="s">
+    <row r="8" ht="72.5" spans="2:5">
+      <c r="B8" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="46" t="s">
         <v>228</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="66" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="24"/>
-    </row>
-    <row r="10" ht="75" spans="2:5">
-      <c r="B10" s="19" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" ht="72.5" spans="2:5">
+      <c r="B10" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="82" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="66" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="11" ht="120" spans="2:5">
-      <c r="B11" s="19" t="s">
+    <row r="11" ht="116" spans="2:5">
+      <c r="B11" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="47" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="12" ht="60" spans="2:5">
-      <c r="B12" s="19" t="s">
+    <row r="12" ht="43.5" spans="2:5">
+      <c r="B12" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="C12"/>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="48" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>242</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E13" s="24"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
@@ -7865,61 +7969,61 @@
       <c r="C14" t="s">
         <v>245</v>
       </c>
-      <c r="E14" s="24"/>
-    </row>
-    <row r="15" ht="75" spans="2:5">
-      <c r="B15" s="19" t="s">
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" ht="72.5" spans="2:5">
+      <c r="B15" s="18" t="s">
         <v>246</v>
       </c>
       <c r="C15" t="s">
         <v>247</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="E15" s="24"/>
-    </row>
-    <row r="16" ht="30" spans="2:5">
-      <c r="B16" s="19" t="s">
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" ht="29" spans="2:5">
+      <c r="B16" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" ht="60" spans="2:5">
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" ht="58" spans="2:5">
       <c r="B17" t="s">
         <v>251</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" t="s">
         <v>254</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E18" s="24"/>
-    </row>
-    <row r="19" ht="30" spans="2:5">
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" ht="29" spans="2:5">
       <c r="B19" t="s">
         <v>256</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="23" t="s">
         <v>259</v>
       </c>
     </row>
@@ -7927,11 +8031,11 @@
       <c r="B20" t="s">
         <v>260</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="24" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="23" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7939,11 +8043,11 @@
       <c r="B21" t="s">
         <v>263</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="24" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="23" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7951,55 +8055,55 @@
       <c r="B22" t="s">
         <v>265</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="24" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="23" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" ht="30" spans="2:5">
+    <row r="23" ht="29" spans="2:5">
       <c r="B23" t="s">
         <v>266</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="24" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="23" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="24" ht="75" spans="2:5">
+    <row r="24" ht="72.5" spans="2:5">
       <c r="B24" t="s">
         <v>268</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>270</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="24"/>
-    </row>
-    <row r="26" ht="60" spans="2:5">
+      <c r="D25" s="11"/>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" ht="58" spans="2:5">
       <c r="B26" t="s">
         <v>272</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="23" t="s">
         <v>275</v>
       </c>
     </row>
@@ -8007,35 +8111,35 @@
       <c r="B27" t="s">
         <v>276</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="24" t="s">
+      <c r="D27" s="11"/>
+      <c r="E27" s="23" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="2:5">
-      <c r="B28" s="12" t="s">
+    <row r="28" ht="15" customHeight="1" spans="2:5">
+      <c r="B28" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="E28" s="24"/>
-    </row>
-    <row r="29" ht="30" spans="2:5">
-      <c r="B29" s="12" t="s">
+      <c r="E28" s="23"/>
+    </row>
+    <row r="29" ht="29" spans="2:5">
+      <c r="B29" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8059,357 +8163,362 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="19.4285714285714" style="35" customWidth="1"/>
-    <col min="2" max="2" width="37" style="35" customWidth="1"/>
-    <col min="3" max="3" width="50.5714285714286" style="35" customWidth="1"/>
-    <col min="4" max="4" width="39.1428571428571" style="35" customWidth="1"/>
-    <col min="5" max="5" width="54.1428571428571" style="35" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="9.14285714285714" style="35"/>
+    <col min="1" max="1" width="19.4272727272727" style="29" customWidth="1"/>
+    <col min="2" max="2" width="37" style="29" customWidth="1"/>
+    <col min="3" max="3" width="50.5727272727273" style="29" customWidth="1"/>
+    <col min="4" max="4" width="39.1454545454545" style="29" customWidth="1"/>
+    <col min="5" max="5" width="54.1454545454545" style="29" customWidth="1"/>
+    <col min="6" max="6" width="51.1454545454545" style="29" customWidth="1"/>
+    <col min="7" max="16384" width="9.14545454545454" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="30" t="s">
         <v>36</v>
       </c>
+      <c r="F1" s="31" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="E3" s="38"/>
+      <c r="C3" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="37"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="38"/>
-    </row>
-    <row r="6" ht="30" spans="2:5">
-      <c r="B6" s="39" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" ht="29" spans="2:5">
+      <c r="B6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="38"/>
-    </row>
-    <row r="7" ht="30" spans="2:6">
-      <c r="B7" s="42" t="s">
+      <c r="C6" s="33" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44" t="s">
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" ht="29" spans="2:6">
+      <c r="B7" s="34" t="s">
         <v>283</v>
       </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35" t="s">
+        <v>284</v>
+      </c>
       <c r="E7" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="F7" s="45"/>
-    </row>
-    <row r="8" ht="195" spans="2:5">
-      <c r="B8" s="40" t="s">
         <v>285</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" ht="188.5" spans="2:5">
+      <c r="B8" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="37" t="s">
         <v>287</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="33" t="s">
         <v>288</v>
       </c>
+      <c r="E8" s="12" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="40" t="s">
-        <v>289</v>
-      </c>
-      <c r="C9" s="47" t="s">
+      <c r="B9" s="29" t="s">
         <v>290</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="38"/>
+      <c r="C9" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="39" t="s">
-        <v>291</v>
-      </c>
-      <c r="C10" s="47" t="s">
+      <c r="B10" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="38"/>
-    </row>
-    <row r="11" ht="30" spans="2:5">
-      <c r="B11" s="39" t="s">
+      <c r="C10" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="38"/>
-    </row>
-    <row r="12" ht="30" spans="2:5">
-      <c r="B12" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="C12" s="47" t="s">
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="33" t="s">
         <v>295</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="38"/>
-    </row>
-    <row r="13" ht="225" spans="2:5">
-      <c r="B13" s="40" t="s">
+      <c r="C12" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="D12" s="33"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" ht="217.5" spans="2:5">
+      <c r="B13" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="C13" s="37" t="s">
         <v>298</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="D13" s="33" t="s">
         <v>299</v>
       </c>
+      <c r="E13" s="38" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="40" t="s">
-        <v>300</v>
-      </c>
-      <c r="C14" s="47" t="s">
+      <c r="B14" s="29" t="s">
         <v>301</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="38"/>
+      <c r="C14" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="32"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="39" t="s">
-        <v>302</v>
-      </c>
-      <c r="C15" s="47" t="s">
+      <c r="B15" s="33" t="s">
         <v>303</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="38"/>
-    </row>
-    <row r="16" ht="30" spans="2:5">
-      <c r="B16" s="39" t="s">
+      <c r="C15" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="D15" s="33"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="38"/>
-    </row>
-    <row r="17" ht="30" spans="2:5">
-      <c r="B17" s="39" t="s">
-        <v>305</v>
-      </c>
-      <c r="C17" s="47" t="s">
+      <c r="D16" s="33"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="33" t="s">
         <v>306</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="38"/>
-    </row>
-    <row r="18" ht="30" spans="2:5">
-      <c r="B18" s="49" t="s">
+      <c r="C17" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="D17" s="33"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" ht="29" spans="2:5">
+      <c r="B18" s="39" t="s">
         <v>308</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="C18" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="D18" s="33" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="19" ht="135" spans="2:5">
-      <c r="B19" s="44" t="s">
+      <c r="E18" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52" t="s">
+    </row>
+    <row r="19" ht="130.5" spans="2:5">
+      <c r="B19" s="35" t="s">
         <v>312</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="C19" s="41"/>
+      <c r="D19" s="42" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="20" ht="60" spans="2:5">
-      <c r="B20" s="39" t="s">
+      <c r="E19" s="32" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" ht="58" spans="2:5">
+      <c r="B20" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="54" t="s">
-        <v>314</v>
-      </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="83" t="s">
+      <c r="C20" s="43" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="21" ht="180" spans="2:5">
-      <c r="B21" s="39" t="s">
+      <c r="D20" s="33"/>
+      <c r="E20" s="67" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" ht="174" spans="2:5">
+      <c r="B21" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="54" t="s">
-        <v>316</v>
-      </c>
-      <c r="D21" s="39" t="s">
+      <c r="C21" s="43" t="s">
         <v>317</v>
       </c>
-      <c r="E21" s="38"/>
-    </row>
-    <row r="22" ht="75" spans="2:5">
-      <c r="B22" s="39" t="s">
+      <c r="D21" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" ht="72.5" spans="2:6">
+      <c r="B22" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="54" t="s">
-        <v>318</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="83" t="s">
+      <c r="C22" s="43" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="23" ht="30" spans="2:5">
-      <c r="B23" s="39" t="s">
+      <c r="D22" s="33"/>
+      <c r="E22" s="67" t="s">
+        <v>320</v>
+      </c>
+      <c r="F22" s="44"/>
+    </row>
+    <row r="23" ht="29" spans="2:5">
+      <c r="B23" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="55" t="s">
-        <v>320</v>
-      </c>
-      <c r="D23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>321</v>
       </c>
-      <c r="E23" s="38"/>
-    </row>
-    <row r="24" ht="75" spans="2:5">
-      <c r="B24" s="39" t="s">
+      <c r="D23" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" ht="72.5" spans="2:6">
+      <c r="B24" s="33" t="s">
         <v>323</v>
       </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="83" t="s">
+      <c r="C24" s="43" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="25" ht="45" spans="2:5">
-      <c r="B25" s="39" t="s">
+      <c r="D24" s="33"/>
+      <c r="E24" s="67" t="s">
+        <v>325</v>
+      </c>
+      <c r="F24" s="44"/>
+    </row>
+    <row r="25" ht="43.5" spans="2:5">
+      <c r="B25" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="55" t="s">
-        <v>325</v>
-      </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="38"/>
+      <c r="C25" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="54" t="s">
-        <v>326</v>
-      </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="38"/>
+      <c r="C26" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D26" s="33"/>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="54" t="s">
-        <v>327</v>
-      </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="38"/>
+      <c r="C27" s="43" t="s">
+        <v>328</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="54" t="s">
-        <v>328</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="38"/>
+      <c r="C28" s="43" t="s">
+        <v>329</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="32"/>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="54" t="s">
-        <v>329</v>
-      </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="38"/>
-    </row>
-    <row r="30" customHeight="1" spans="2:5">
-      <c r="B30" s="39" t="s">
+      <c r="C29" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" ht="15" customHeight="1" spans="2:5">
+      <c r="B30" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="39" t="s">
-        <v>330</v>
-      </c>
-      <c r="E30" s="38"/>
-    </row>
-    <row r="31" ht="30" spans="2:5">
-      <c r="B31" s="39" t="s">
+      <c r="D30" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" ht="29" spans="2:5">
+      <c r="B31" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="C31" s="55" t="s">
-        <v>331</v>
-      </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="38"/>
+      <c r="C31" s="45" t="s">
+        <v>332</v>
+      </c>
+      <c r="D31" s="33"/>
+      <c r="E31" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8435,329 +8544,329 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.2190476190476" customWidth="1"/>
-    <col min="2" max="2" width="26.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="43.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="47.2857142857143" customWidth="1"/>
-    <col min="5" max="5" width="80.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
+    <col min="1" max="1" width="13.2181818181818" customWidth="1"/>
+    <col min="2" max="2" width="26.2818181818182" customWidth="1"/>
+    <col min="3" max="3" width="43.7181818181818" customWidth="1"/>
+    <col min="4" max="4" width="47.2818181818182" customWidth="1"/>
+    <col min="5" max="5" width="80.5727272727273" customWidth="1"/>
+    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" ht="45" spans="2:5">
-      <c r="B4" s="12" t="s">
+      <c r="C3" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="E4" s="12"/>
+      <c r="D4" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" ht="30" spans="2:5">
-      <c r="B6" s="20" t="s">
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" ht="29" spans="2:5">
+      <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="E6" s="12"/>
+      <c r="C6" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="8" ht="150" spans="2:5">
-      <c r="B8" s="20" t="s">
+      <c r="E7" s="20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" ht="145" spans="2:5">
+      <c r="B8" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>337</v>
       </c>
+      <c r="D8" s="11" t="s">
+        <v>338</v>
+      </c>
       <c r="E8" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="9" ht="120" spans="2:5">
-      <c r="B9" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28" t="s">
+    </row>
+    <row r="9" ht="116" spans="2:5">
+      <c r="B9" s="25" t="s">
         <v>340</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="27" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="10" ht="45" spans="1:5">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30" t="s">
+      <c r="E9" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="10" ht="43.5" spans="1:5">
+      <c r="A10" s="26"/>
+      <c r="B10" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="D10" s="28"/>
+      <c r="C10" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D10" s="27"/>
       <c r="E10" s="8" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="11" ht="210" spans="1:5">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="11" ht="203" spans="1:5">
+      <c r="A11" s="26"/>
+      <c r="B11" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="28"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="12" ht="210" spans="1:5">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" ht="203" spans="1:5">
+      <c r="A12" s="26"/>
+      <c r="B12" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="28"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30" t="s">
-        <v>346</v>
-      </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="28"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="8" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="14" ht="150" spans="2:5">
-      <c r="B14" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="C14" s="12" t="s">
+    </row>
+    <row r="14" ht="130.5" spans="2:5">
+      <c r="B14" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="D14" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="20" t="s">
-        <v>351</v>
-      </c>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="C15" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="20" t="s">
-        <v>353</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="B16" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" ht="105" spans="2:5">
-      <c r="B18" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" ht="101.5" spans="2:5">
+      <c r="B18" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="19" ht="30" spans="2:5">
-      <c r="B19" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="20" ht="30" spans="2:5">
-      <c r="B20" s="12" t="s">
+    </row>
+    <row r="19" ht="29" spans="2:5">
+      <c r="B19" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="21" ht="75" spans="2:5">
-      <c r="B21" s="20" t="s">
+      <c r="C19" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" ht="29" spans="2:5">
+      <c r="B20" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" ht="72.5" spans="2:5">
+      <c r="B21" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" ht="30" spans="2:5">
-      <c r="B22" s="20" t="s">
+      <c r="D21" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" ht="29" spans="2:5">
+      <c r="B22" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" ht="45" spans="2:5">
-      <c r="B23" s="26" t="s">
-        <v>364</v>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" ht="43.5" spans="2:5">
+      <c r="B23" s="25" t="s">
+        <v>365</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="D23" s="28" t="s">
         <v>366</v>
       </c>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" ht="30" spans="2:5">
-      <c r="B24" s="20" t="s">
+      <c r="D23" s="27" t="s">
         <v>367</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="19" t="s">
         <v>368</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="25" ht="60" spans="2:5">
-      <c r="B25" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>371</v>
+      </c>
+    </row>
+    <row r="25" ht="58" spans="2:5">
+      <c r="B25" s="11" t="s">
+        <v>372</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" ht="30" spans="2:5">
-      <c r="B26" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" ht="29" spans="2:5">
+      <c r="B26" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="D26" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="E27" s="12"/>
+      <c r="D27" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" ht="78" customHeight="1" spans="2:5">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C28" s="34" t="s">
-        <v>377</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="C28" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8787,227 +8896,227 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="22.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="22.2818181818182" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="70.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="47.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="49.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
+    <col min="3" max="3" width="70.2818181818182" customWidth="1"/>
+    <col min="4" max="4" width="47.1454545454545" customWidth="1"/>
+    <col min="5" max="5" width="49.5727272727273" customWidth="1"/>
+    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" ht="30" spans="1:5">
-      <c r="A2" s="23" t="s">
-        <v>378</v>
-      </c>
-      <c r="E2" s="24"/>
+    <row r="2" ht="29" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="E3" s="24"/>
+      <c r="C3" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>379</v>
-      </c>
-      <c r="E4" s="24"/>
+        <v>380</v>
+      </c>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="24"/>
-    </row>
-    <row r="6" ht="30" spans="2:5">
-      <c r="B6" s="20" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" ht="29" spans="2:5">
+      <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" ht="150" spans="2:5">
-      <c r="B7" s="19" t="s">
+      <c r="C6" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" ht="145" spans="2:5">
+      <c r="B7" s="18" t="s">
         <v>179</v>
       </c>
       <c r="C7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="19" t="s">
-        <v>348</v>
+      <c r="B8" s="18" t="s">
+        <v>349</v>
       </c>
       <c r="C8" t="s">
-        <v>382</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="24"/>
+        <v>383</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" ht="42.95" customHeight="1" spans="2:5">
-      <c r="B9" s="19" t="s">
-        <v>351</v>
+      <c r="B9" s="18" t="s">
+        <v>352</v>
       </c>
       <c r="C9" t="s">
-        <v>383</v>
-      </c>
-      <c r="D9" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="E9" s="24"/>
+      <c r="D9" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" ht="60.95" customHeight="1" spans="2:5">
-      <c r="B11" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="24"/>
-    </row>
-    <row r="12" ht="30" spans="2:5">
-      <c r="B12" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="B11" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" ht="29" spans="2:5">
+      <c r="B12" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13" ht="30" spans="2:5">
-      <c r="B13" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="24"/>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" ht="29" spans="2:5">
+      <c r="B13" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" ht="78" customHeight="1" spans="2:5">
-      <c r="B14" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>389</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="24"/>
-    </row>
-    <row r="15" ht="45" spans="2:5">
-      <c r="B15" s="19" t="s">
+      <c r="B14" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" ht="43.5" spans="2:5">
+      <c r="B15" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>390</v>
-      </c>
-      <c r="E15" s="24"/>
+      <c r="C15" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" ht="30" spans="2:5">
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" ht="29" spans="2:5">
       <c r="B17" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C17" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D17" t="s">
-        <v>369</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="18" customHeight="1" spans="2:5">
-      <c r="B18" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="2:5">
+      <c r="B18" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="E18" s="24"/>
+      <c r="D18" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>377</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="24"/>
+      <c r="C19" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9029,195 +9138,195 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" customWidth="1"/>
-    <col min="2" max="2" width="23.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="34.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="25.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="33.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
+    <col min="1" max="1" width="9.14545454545454" customWidth="1"/>
+    <col min="2" max="2" width="23.1454545454545" customWidth="1"/>
+    <col min="3" max="3" width="34.2818181818182" customWidth="1"/>
+    <col min="4" max="4" width="25.1454545454545" customWidth="1"/>
+    <col min="5" max="5" width="33.4272727272727" customWidth="1"/>
+    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>394</v>
+      <c r="C3" s="11" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" ht="45" spans="2:5">
-      <c r="B6" s="20" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" ht="29" spans="2:5">
+      <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="C6" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>397</v>
+      <c r="C7" s="11" t="s">
+        <v>398</v>
       </c>
       <c r="D7" t="s">
-        <v>398</v>
-      </c>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" ht="165" spans="2:5">
-      <c r="B8" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="C8" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" ht="159.5" spans="2:5">
+      <c r="B8" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="19" t="s">
-        <v>351</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>400</v>
+      <c r="B9" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>401</v>
+      <c r="B10" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>354</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="12" ht="90" spans="2:4">
-      <c r="B12" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" ht="87" spans="2:4">
+      <c r="B12" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>403</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="13" ht="45" spans="2:3">
-      <c r="B13" s="19" t="s">
+    <row r="13" ht="29" spans="2:3">
+      <c r="B13" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="14" ht="75" spans="2:4">
-      <c r="B14" s="19" t="s">
-        <v>364</v>
-      </c>
-      <c r="C14" s="12" t="s">
+    <row r="14" ht="72.5" spans="2:4">
+      <c r="B14" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="15" ht="90" spans="2:4">
+      <c r="C14" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="15" ht="87" spans="2:4">
       <c r="B15" t="s">
-        <v>405</v>
-      </c>
-      <c r="C15" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>407</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>408</v>
-      </c>
-      <c r="C16" s="12" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="17" customHeight="1" spans="2:4">
-      <c r="B17" s="12" t="s">
+      <c r="C16" s="11" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="2:4">
+      <c r="B17" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="18" ht="30" spans="2:4">
-      <c r="B18" s="12" t="s">
+      <c r="D17" s="11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" ht="29" spans="2:4">
+      <c r="B18" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>411</v>
-      </c>
-      <c r="D18" s="12"/>
+      <c r="C18" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="D18" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
docs: update HL7 to FHIR Conversion document with the changes in Consent resource.
</commit_message>
<xml_diff>
--- a/support/specifications/hl7/HL7v2.to.FHIR.Conversion.Spec.xlsx
+++ b/support/specifications/hl7/HL7v2.to.FHIR.Conversion.Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="8000" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -1791,7 +1791,46 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>' can be taken as the Consent resource.</t>
+      <t xml:space="preserve">' can be taken as the Consent resource.
+If there is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>NO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> OBX segment in which OBX-3.1 = '105511-0' or OBX.3.2 = 'AHC-HRSN Patient Consent'  then, the Consent resource will be generated with 'provision.type' as '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>deny</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>' and the 'Consent Source' will be 'TechBD Generated'.</t>
     </r>
   </si>
   <si>
@@ -2212,7 +2251,66 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>".</t>
+      <t xml:space="preserve">".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>:
+If there is NO OBX segment in which OBX-3.1 = '105511-0' or OBX.3.2 = 'AHC-HRSN Patient Consent'  then, the Consent resource will be generated with 'provision.type' as '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>deny</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>' and the 'Consent Source' will be '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TechBD Generated</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>'.</t>
     </r>
   </si>
   <si>
@@ -5119,9 +5217,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -5135,7 +5241,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -5146,27 +5265,6 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -5850,7 +5948,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5970,7 +6068,7 @@
     <cellStyle name="Warning" xfId="59"/>
   </cellStyles>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{79655ED8-46CF-41F3-B049-9A522ABE8835}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{AADC0999-BA12-42CC-B1B0-98753EE1D3E7}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6238,86 +6336,83 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C14"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8545454545455" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11.8571428571429" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="14.2818181818182" style="64" customWidth="1"/>
+    <col min="1" max="1" width="14.2857142857143" style="64" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="123.572727272727" customWidth="1"/>
+    <col min="3" max="3" width="123.571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" s="18"/>
+    <row r="1" spans="1:3">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="60"/>
+      <c r="B2" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="60"/>
+      <c r="B3" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="60"/>
+      <c r="B4" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" ht="45" spans="1:3">
+      <c r="A5" s="60"/>
+      <c r="B5" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="60"/>
+      <c r="B6" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="A7" s="60"/>
+      <c r="B7" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="60"/>
-      <c r="B8" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="60"/>
-      <c r="B9" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="60"/>
-      <c r="B10" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" ht="43.5" spans="1:3">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="60"/>
-      <c r="B12" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
+      <c r="B8" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1.39370078740157" bottom="1.39370078740157" header="1" footer="1"/>
@@ -6337,15 +6432,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7181818181818" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.5727272727273" style="2" customWidth="1"/>
-    <col min="3" max="3" width="49.6636363636364" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.5545454545455" style="2" customWidth="1"/>
-    <col min="5" max="5" width="53.2818181818182" style="2" customWidth="1"/>
-    <col min="6" max="6" width="47.5727272727273" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.14545454545454" style="2"/>
+    <col min="1" max="1" width="14.7142857142857" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.5714285714286" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.6666666666667" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.552380952381" style="2" customWidth="1"/>
+    <col min="5" max="5" width="53.2857142857143" style="2" customWidth="1"/>
+    <col min="6" max="6" width="47.5714285714286" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6411,7 +6506,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" s="2" customFormat="1" ht="29" spans="2:6">
+    <row r="6" s="2" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
@@ -6437,7 +6532,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="1" ht="145" spans="2:5">
+    <row r="8" s="2" customFormat="1" ht="150" spans="2:5">
       <c r="B8" s="6" t="s">
         <v>179</v>
       </c>
@@ -6463,7 +6558,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" ht="145" spans="2:5">
+    <row r="10" s="2" customFormat="1" ht="150" spans="2:5">
       <c r="B10" s="6" t="s">
         <v>349</v>
       </c>
@@ -6477,7 +6572,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="1" ht="159.5" spans="2:5">
+    <row r="11" s="2" customFormat="1" ht="180" spans="2:5">
       <c r="B11" s="6" t="s">
         <v>352</v>
       </c>
@@ -6487,7 +6582,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" ht="145" spans="2:5">
+    <row r="12" s="2" customFormat="1" ht="150" spans="2:5">
       <c r="B12" s="6" t="s">
         <v>354</v>
       </c>
@@ -6497,7 +6592,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="1" ht="58" spans="2:4">
+    <row r="13" s="2" customFormat="1" ht="75" spans="2:4">
       <c r="B13" s="6" t="s">
         <v>246</v>
       </c>
@@ -6508,7 +6603,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="14" s="2" customFormat="1" ht="29" spans="2:3">
+    <row r="14" s="2" customFormat="1" ht="30" spans="2:3">
       <c r="B14" s="6" t="s">
         <v>249</v>
       </c>
@@ -6516,7 +6611,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" s="2" customFormat="1" ht="43.5" spans="2:4">
+    <row r="15" s="2" customFormat="1" ht="45" spans="2:4">
       <c r="B15" s="6" t="s">
         <v>365</v>
       </c>
@@ -6527,7 +6622,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="16" s="2" customFormat="1" ht="29" spans="2:5">
+    <row r="16" s="2" customFormat="1" ht="30" spans="2:5">
       <c r="B16" s="6" t="s">
         <v>368</v>
       </c>
@@ -6541,7 +6636,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="17" s="2" customFormat="1" ht="43.5" spans="2:4">
+    <row r="17" s="2" customFormat="1" ht="45" spans="2:4">
       <c r="B17" s="6" t="s">
         <v>428</v>
       </c>
@@ -6565,7 +6660,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" ht="159.5" spans="2:5">
+    <row r="19" s="2" customFormat="1" ht="165" spans="2:5">
       <c r="B19" s="2" t="s">
         <v>431</v>
       </c>
@@ -6617,12 +6712,12 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="14.7181818181818" style="60" customWidth="1"/>
-    <col min="2" max="2" width="28.2818181818182" style="60" customWidth="1"/>
-    <col min="3" max="3" width="66.4272727272727" style="60" customWidth="1"/>
-    <col min="4" max="4" width="46.2818181818182" style="60" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" style="60" customWidth="1"/>
+    <col min="2" max="2" width="28.2857142857143" style="60" customWidth="1"/>
+    <col min="3" max="3" width="66.4285714285714" style="60" customWidth="1"/>
+    <col min="4" max="4" width="46.2857142857143" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6665,7 +6760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" ht="87" spans="2:4">
+    <row r="5" ht="90" spans="2:4">
       <c r="B5" s="60" t="s">
         <v>23</v>
       </c>
@@ -6702,7 +6797,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" ht="29" spans="2:3">
+    <row r="9" ht="30" spans="2:3">
       <c r="B9" s="60" t="s">
         <v>32</v>
       </c>
@@ -6772,20 +6867,20 @@
   <sheetPr/>
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.1181818181818" customWidth="1"/>
-    <col min="2" max="2" width="39.1454545454545" style="11" customWidth="1"/>
-    <col min="3" max="3" width="61.5727272727273" style="11" customWidth="1"/>
-    <col min="4" max="4" width="66.8545454545455" style="11" customWidth="1"/>
-    <col min="5" max="5" width="64.5727272727273" style="11" customWidth="1"/>
-    <col min="6" max="256" width="11.8545454545455" customWidth="1"/>
+    <col min="1" max="1" width="13.1142857142857" customWidth="1"/>
+    <col min="2" max="2" width="39.1428571428571" style="11" customWidth="1"/>
+    <col min="3" max="3" width="61.5714285714286" style="11" customWidth="1"/>
+    <col min="4" max="4" width="66.8571428571429" style="11" customWidth="1"/>
+    <col min="5" max="5" width="64.5714285714286" style="11" customWidth="1"/>
+    <col min="6" max="256" width="11.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="1" spans="1:5">
@@ -6843,7 +6938,7 @@
       </c>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" ht="30" spans="2:5">
       <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
@@ -6852,7 +6947,7 @@
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" ht="58" spans="2:5">
+    <row r="7" ht="60" spans="2:5">
       <c r="B7" s="11" t="s">
         <v>41</v>
       </c>
@@ -6866,7 +6961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" ht="58" spans="2:5">
+    <row r="8" ht="60" spans="2:5">
       <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
@@ -6923,7 +7018,7 @@
       </c>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" ht="58" spans="2:5">
+    <row r="13" ht="60" spans="2:5">
       <c r="B13" s="11" t="s">
         <v>58</v>
       </c>
@@ -6935,7 +7030,7 @@
       </c>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" ht="29" spans="2:5">
+    <row r="14" ht="30" spans="2:5">
       <c r="B14" s="11" t="s">
         <v>61</v>
       </c>
@@ -6971,7 +7066,7 @@
       </c>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" ht="116" spans="2:5">
+    <row r="17" ht="120" spans="2:5">
       <c r="B17" s="11" t="s">
         <v>70</v>
       </c>
@@ -6983,7 +7078,7 @@
       </c>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" ht="29" spans="2:5">
+    <row r="18" ht="30" spans="2:5">
       <c r="B18" s="11" t="s">
         <v>73</v>
       </c>
@@ -7046,7 +7141,7 @@
       </c>
       <c r="E24" s="23"/>
     </row>
-    <row r="25" ht="72.5" spans="2:5">
+    <row r="25" ht="75" spans="2:5">
       <c r="B25" s="11" t="s">
         <v>87</v>
       </c>
@@ -7058,7 +7153,7 @@
       </c>
       <c r="E25" s="23"/>
     </row>
-    <row r="26" ht="29" spans="2:5">
+    <row r="26" ht="45" spans="2:5">
       <c r="B26" s="27" t="s">
         <v>90</v>
       </c>
@@ -7072,7 +7167,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" ht="29" spans="2:5">
+    <row r="27" ht="30" spans="2:5">
       <c r="B27" s="27" t="s">
         <v>94</v>
       </c>
@@ -7082,7 +7177,7 @@
       <c r="D27" s="56"/>
       <c r="E27" s="57"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" ht="30" spans="2:5">
       <c r="B28" s="27" t="s">
         <v>96</v>
       </c>
@@ -7092,7 +7187,7 @@
       <c r="D28" s="56"/>
       <c r="E28" s="57"/>
     </row>
-    <row r="29" ht="29" spans="2:5">
+    <row r="29" ht="30" spans="2:5">
       <c r="B29" s="27" t="s">
         <v>98</v>
       </c>
@@ -7112,7 +7207,7 @@
       <c r="D30" s="56"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" ht="29" spans="2:5">
+    <row r="31" ht="30" spans="2:5">
       <c r="B31" s="27" t="s">
         <v>90</v>
       </c>
@@ -7126,7 +7221,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" ht="29" spans="2:5">
+    <row r="32" ht="30" spans="2:5">
       <c r="B32" s="27" t="s">
         <v>94</v>
       </c>
@@ -7136,7 +7231,7 @@
       <c r="D32" s="56"/>
       <c r="E32" s="57"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" ht="30" spans="2:5">
       <c r="B33" s="27" t="s">
         <v>96</v>
       </c>
@@ -7146,7 +7241,7 @@
       <c r="D33" s="56"/>
       <c r="E33" s="57"/>
     </row>
-    <row r="34" ht="29" spans="2:5">
+    <row r="34" ht="30" spans="2:5">
       <c r="B34" s="27" t="s">
         <v>98</v>
       </c>
@@ -7178,7 +7273,7 @@
       </c>
       <c r="E36" s="57"/>
     </row>
-    <row r="37" ht="43.5" spans="2:5">
+    <row r="37" ht="45" spans="2:5">
       <c r="B37" s="27" t="s">
         <v>109</v>
       </c>
@@ -7190,7 +7285,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" ht="130.5" spans="2:5">
+    <row r="38" ht="135" spans="2:5">
       <c r="B38" s="58" t="s">
         <v>112</v>
       </c>
@@ -7202,7 +7297,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" ht="130.5" spans="2:5">
+    <row r="39" ht="135" spans="2:5">
       <c r="B39" s="58" t="s">
         <v>115</v>
       </c>
@@ -7250,7 +7345,7 @@
       </c>
       <c r="E43" s="23"/>
     </row>
-    <row r="44" ht="188.5" spans="2:5">
+    <row r="44" ht="195" spans="2:5">
       <c r="B44" s="19" t="s">
         <v>124</v>
       </c>
@@ -7262,7 +7357,7 @@
       </c>
       <c r="E44" s="23"/>
     </row>
-    <row r="45" ht="188.5" spans="2:5">
+    <row r="45" ht="195" spans="2:5">
       <c r="B45" s="19" t="s">
         <v>127</v>
       </c>
@@ -7276,7 +7371,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" ht="188.5" spans="2:5">
+    <row r="46" ht="195" spans="2:5">
       <c r="B46" s="19" t="s">
         <v>131</v>
       </c>
@@ -7324,7 +7419,7 @@
       </c>
       <c r="E50" s="23"/>
     </row>
-    <row r="51" ht="145" spans="2:5">
+    <row r="51" ht="150" spans="2:5">
       <c r="B51" s="11" t="s">
         <v>140</v>
       </c>
@@ -7392,7 +7487,7 @@
       </c>
       <c r="E57" s="23"/>
     </row>
-    <row r="58" ht="174" spans="2:5">
+    <row r="58" ht="180" spans="2:5">
       <c r="B58" s="11" t="s">
         <v>154</v>
       </c>
@@ -7404,7 +7499,7 @@
       </c>
       <c r="E58" s="23"/>
     </row>
-    <row r="59" ht="72.5" spans="2:5">
+    <row r="59" ht="90" spans="2:5">
       <c r="B59" s="27" t="s">
         <v>157</v>
       </c>
@@ -7414,7 +7509,7 @@
       </c>
       <c r="E59" s="23"/>
     </row>
-    <row r="60" ht="246.5" spans="2:5">
+    <row r="60" ht="255" spans="2:5">
       <c r="B60" s="11" t="s">
         <v>159</v>
       </c>
@@ -7428,7 +7523,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" ht="130.5" spans="2:5">
+    <row r="61" ht="135" spans="2:5">
       <c r="B61" s="11" t="s">
         <v>163</v>
       </c>
@@ -7440,7 +7535,7 @@
       </c>
       <c r="E61" s="23"/>
     </row>
-    <row r="62" spans="2:5">
+    <row r="62" ht="30" spans="2:5">
       <c r="B62" s="11" t="s">
         <v>166</v>
       </c>
@@ -7505,20 +7600,20 @@
   <sheetPr/>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.14545454545454" customWidth="1"/>
-    <col min="2" max="2" width="40.8545454545455" customWidth="1"/>
-    <col min="3" max="3" width="61.5727272727273" customWidth="1"/>
-    <col min="4" max="4" width="57.4272727272727" customWidth="1"/>
-    <col min="5" max="5" width="54.8545454545455" customWidth="1"/>
-    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
+    <col min="1" max="1" width="9.14285714285714" customWidth="1"/>
+    <col min="2" max="2" width="40.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="61.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="57.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="54.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7538,7 +7633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" ht="31" customHeight="1" spans="1:5">
       <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
@@ -7547,7 +7642,7 @@
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
-      <c r="E2" s="23"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="11" t="s">
@@ -7585,7 +7680,7 @@
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" ht="29" spans="2:5">
+    <row r="7" ht="45" spans="2:5">
       <c r="B7" s="18" t="s">
         <v>179</v>
       </c>
@@ -7599,7 +7694,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" ht="130.5" spans="2:5">
+    <row r="8" ht="135" spans="2:5">
       <c r="B8" s="51" t="s">
         <v>183</v>
       </c>
@@ -7635,7 +7730,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" ht="217.5" spans="2:5">
+    <row r="11" ht="225" spans="2:5">
       <c r="B11" s="18" t="s">
         <v>192</v>
       </c>
@@ -7671,7 +7766,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" ht="29" spans="2:5">
+    <row r="14" ht="30" spans="2:5">
       <c r="B14" s="18" t="s">
         <v>199</v>
       </c>
@@ -7685,7 +7780,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" ht="43.5" spans="2:5">
+    <row r="15" ht="120" spans="2:5">
       <c r="B15" s="18" t="s">
         <v>203</v>
       </c>
@@ -7699,7 +7794,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" ht="43.5" spans="2:5">
+    <row r="16" ht="45" spans="2:5">
       <c r="B16" s="18" t="s">
         <v>207</v>
       </c>
@@ -7711,7 +7806,7 @@
       </c>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" ht="58" spans="2:5">
+    <row r="17" ht="60" spans="2:5">
       <c r="B17" s="51" t="s">
         <v>210</v>
       </c>
@@ -7723,7 +7818,7 @@
       </c>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" ht="58" spans="2:5">
+    <row r="18" ht="60" spans="2:5">
       <c r="B18" s="54" t="s">
         <v>213</v>
       </c>
@@ -7787,7 +7882,7 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B2:E2"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D21:D22"/>
   </mergeCells>
@@ -7807,14 +7902,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.14545454545454" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="43.5727272727273" customWidth="1"/>
-    <col min="5" max="5" width="57.5727272727273" customWidth="1"/>
-    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
+    <col min="4" max="4" width="43.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="57.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7873,7 +7968,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" ht="29" spans="2:5">
+    <row r="6" ht="30" spans="2:5">
       <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
@@ -7895,7 +7990,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" ht="72.5" spans="2:5">
+    <row r="8" ht="75" spans="2:5">
       <c r="B8" s="18" t="s">
         <v>227</v>
       </c>
@@ -7919,7 +8014,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" ht="72.5" spans="2:5">
+    <row r="10" ht="75" spans="2:5">
       <c r="B10" s="18" t="s">
         <v>233</v>
       </c>
@@ -7931,7 +8026,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" ht="116" spans="2:5">
+    <row r="11" ht="120" spans="2:5">
       <c r="B11" s="18" t="s">
         <v>236</v>
       </c>
@@ -7945,7 +8040,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" ht="43.5" spans="2:5">
+    <row r="12" ht="60" spans="2:5">
       <c r="B12" s="18" t="s">
         <v>240</v>
       </c>
@@ -7971,7 +8066,7 @@
       </c>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" ht="72.5" spans="2:5">
+    <row r="15" ht="75" spans="2:5">
       <c r="B15" s="18" t="s">
         <v>246</v>
       </c>
@@ -7983,7 +8078,7 @@
       </c>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" ht="29" spans="2:5">
+    <row r="16" ht="30" spans="2:5">
       <c r="B16" s="18" t="s">
         <v>249</v>
       </c>
@@ -7992,7 +8087,7 @@
       </c>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" ht="58" spans="2:5">
+    <row r="17" ht="60" spans="2:5">
       <c r="B17" t="s">
         <v>251</v>
       </c>
@@ -8013,7 +8108,7 @@
       </c>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" ht="29" spans="2:5">
+    <row r="19" ht="30" spans="2:5">
       <c r="B19" t="s">
         <v>256</v>
       </c>
@@ -8061,7 +8156,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" ht="29" spans="2:5">
+    <row r="23" ht="30" spans="2:5">
       <c r="B23" t="s">
         <v>266</v>
       </c>
@@ -8073,7 +8168,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" ht="72.5" spans="2:5">
+    <row r="24" ht="75" spans="2:5">
       <c r="B24" t="s">
         <v>268</v>
       </c>
@@ -8093,7 +8188,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="23"/>
     </row>
-    <row r="26" ht="58" spans="2:5">
+    <row r="26" ht="60" spans="2:5">
       <c r="B26" t="s">
         <v>272</v>
       </c>
@@ -8119,7 +8214,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" spans="2:5">
+    <row r="28" customHeight="1" spans="2:5">
       <c r="B28" s="11" t="s">
         <v>170</v>
       </c>
@@ -8131,7 +8226,7 @@
       </c>
       <c r="E28" s="23"/>
     </row>
-    <row r="29" ht="29" spans="2:5">
+    <row r="29" ht="30" spans="2:5">
       <c r="B29" s="11" t="s">
         <v>173</v>
       </c>
@@ -8163,15 +8258,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="19.4272727272727" style="29" customWidth="1"/>
+    <col min="1" max="1" width="19.4285714285714" style="29" customWidth="1"/>
     <col min="2" max="2" width="37" style="29" customWidth="1"/>
-    <col min="3" max="3" width="50.5727272727273" style="29" customWidth="1"/>
-    <col min="4" max="4" width="39.1454545454545" style="29" customWidth="1"/>
-    <col min="5" max="5" width="54.1454545454545" style="29" customWidth="1"/>
-    <col min="6" max="6" width="51.1454545454545" style="29" customWidth="1"/>
-    <col min="7" max="16384" width="9.14545454545454" style="29"/>
+    <col min="3" max="3" width="50.5714285714286" style="29" customWidth="1"/>
+    <col min="4" max="4" width="39.1428571428571" style="29" customWidth="1"/>
+    <col min="5" max="5" width="54.1428571428571" style="29" customWidth="1"/>
+    <col min="6" max="6" width="51.1428571428571" style="29" customWidth="1"/>
+    <col min="7" max="16384" width="9.14285714285714" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8229,7 +8324,7 @@
       <c r="D5" s="33"/>
       <c r="E5" s="32"/>
     </row>
-    <row r="6" ht="29" spans="2:5">
+    <row r="6" ht="30" spans="2:5">
       <c r="B6" s="33" t="s">
         <v>26</v>
       </c>
@@ -8239,7 +8334,7 @@
       <c r="D6" s="33"/>
       <c r="E6" s="32"/>
     </row>
-    <row r="7" ht="29" spans="2:6">
+    <row r="7" ht="30" spans="2:6">
       <c r="B7" s="34" t="s">
         <v>283</v>
       </c>
@@ -8252,7 +8347,7 @@
       </c>
       <c r="F7" s="36"/>
     </row>
-    <row r="8" ht="188.5" spans="2:5">
+    <row r="8" ht="195" spans="2:5">
       <c r="B8" s="29" t="s">
         <v>286</v>
       </c>
@@ -8286,7 +8381,7 @@
       <c r="D10" s="33"/>
       <c r="E10" s="32"/>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" ht="30" spans="2:5">
       <c r="B11" s="33" t="s">
         <v>294</v>
       </c>
@@ -8296,7 +8391,7 @@
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" ht="30" spans="2:5">
       <c r="B12" s="33" t="s">
         <v>295</v>
       </c>
@@ -8306,7 +8401,7 @@
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
     </row>
-    <row r="13" ht="217.5" spans="2:5">
+    <row r="13" ht="225" spans="2:5">
       <c r="B13" s="29" t="s">
         <v>297</v>
       </c>
@@ -8340,7 +8435,7 @@
       <c r="D15" s="33"/>
       <c r="E15" s="32"/>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" ht="30" spans="2:5">
       <c r="B16" s="33" t="s">
         <v>305</v>
       </c>
@@ -8350,7 +8445,7 @@
       <c r="D16" s="33"/>
       <c r="E16" s="32"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" ht="30" spans="2:5">
       <c r="B17" s="33" t="s">
         <v>306</v>
       </c>
@@ -8360,7 +8455,7 @@
       <c r="D17" s="33"/>
       <c r="E17" s="32"/>
     </row>
-    <row r="18" ht="29" spans="2:5">
+    <row r="18" ht="30" spans="2:5">
       <c r="B18" s="39" t="s">
         <v>308</v>
       </c>
@@ -8374,7 +8469,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="19" ht="130.5" spans="2:5">
+    <row r="19" ht="135" spans="2:5">
       <c r="B19" s="35" t="s">
         <v>312</v>
       </c>
@@ -8386,7 +8481,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="20" ht="58" spans="2:5">
+    <row r="20" ht="60" spans="2:5">
       <c r="B20" s="33" t="s">
         <v>83</v>
       </c>
@@ -8398,7 +8493,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="21" ht="174" spans="2:5">
+    <row r="21" ht="180" spans="2:5">
       <c r="B21" s="33" t="s">
         <v>85</v>
       </c>
@@ -8410,7 +8505,7 @@
       </c>
       <c r="E21" s="32"/>
     </row>
-    <row r="22" ht="72.5" spans="2:6">
+    <row r="22" ht="75" spans="2:6">
       <c r="B22" s="33" t="s">
         <v>87</v>
       </c>
@@ -8423,7 +8518,7 @@
       </c>
       <c r="F22" s="44"/>
     </row>
-    <row r="23" ht="29" spans="2:5">
+    <row r="23" ht="30" spans="2:5">
       <c r="B23" s="33" t="s">
         <v>70</v>
       </c>
@@ -8435,7 +8530,7 @@
       </c>
       <c r="E23" s="32"/>
     </row>
-    <row r="24" ht="72.5" spans="2:6">
+    <row r="24" ht="75" spans="2:6">
       <c r="B24" s="33" t="s">
         <v>323</v>
       </c>
@@ -8448,7 +8543,7 @@
       </c>
       <c r="F24" s="44"/>
     </row>
-    <row r="25" ht="43.5" spans="2:5">
+    <row r="25" ht="45" spans="2:5">
       <c r="B25" s="33" t="s">
         <v>73</v>
       </c>
@@ -8498,7 +8593,7 @@
       <c r="D29" s="33"/>
       <c r="E29" s="32"/>
     </row>
-    <row r="30" ht="15" customHeight="1" spans="2:5">
+    <row r="30" customHeight="1" spans="2:5">
       <c r="B30" s="33" t="s">
         <v>170</v>
       </c>
@@ -8510,7 +8605,7 @@
       </c>
       <c r="E30" s="32"/>
     </row>
-    <row r="31" ht="29" spans="2:5">
+    <row r="31" ht="30" spans="2:5">
       <c r="B31" s="33" t="s">
         <v>173</v>
       </c>
@@ -8544,14 +8639,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.2181818181818" customWidth="1"/>
-    <col min="2" max="2" width="26.2818181818182" customWidth="1"/>
-    <col min="3" max="3" width="43.7181818181818" customWidth="1"/>
-    <col min="4" max="4" width="47.2818181818182" customWidth="1"/>
-    <col min="5" max="5" width="80.5727272727273" customWidth="1"/>
-    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
+    <col min="1" max="1" width="13.2190476190476" customWidth="1"/>
+    <col min="2" max="2" width="26.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="43.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="47.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="80.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8607,7 +8702,7 @@
       </c>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" ht="29" spans="2:5">
+    <row r="6" ht="30" spans="2:5">
       <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
@@ -8628,7 +8723,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" ht="145" spans="2:5">
+    <row r="8" ht="150" spans="2:5">
       <c r="B8" s="19" t="s">
         <v>179</v>
       </c>
@@ -8642,7 +8737,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" ht="116" spans="2:5">
+    <row r="9" ht="120" spans="2:5">
       <c r="B9" s="25" t="s">
         <v>340</v>
       </c>
@@ -8654,7 +8749,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="10" ht="43.5" spans="1:5">
+    <row r="10" ht="45" spans="1:5">
       <c r="A10" s="26"/>
       <c r="B10" s="6" t="s">
         <v>197</v>
@@ -8667,7 +8762,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="11" ht="203" spans="1:5">
+    <row r="11" ht="210" spans="1:5">
       <c r="A11" s="26"/>
       <c r="B11" s="6" t="s">
         <v>192</v>
@@ -8678,7 +8773,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" ht="203" spans="1:5">
+    <row r="12" ht="210" spans="1:5">
       <c r="A12" s="26"/>
       <c r="B12" s="6" t="s">
         <v>195</v>
@@ -8700,7 +8795,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" ht="130.5" spans="2:5">
+    <row r="14" ht="150" spans="2:5">
       <c r="B14" s="11" t="s">
         <v>349</v>
       </c>
@@ -8739,7 +8834,7 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" ht="101.5" spans="2:5">
+    <row r="18" ht="105" spans="2:5">
       <c r="B18" s="11" t="s">
         <v>357</v>
       </c>
@@ -8753,7 +8848,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="19" ht="29" spans="2:5">
+    <row r="19" ht="30" spans="2:5">
       <c r="B19" s="11" t="s">
         <v>361</v>
       </c>
@@ -8764,7 +8859,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" ht="29" spans="2:5">
+    <row r="20" ht="30" spans="2:5">
       <c r="B20" s="11" t="s">
         <v>362</v>
       </c>
@@ -8775,7 +8870,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" ht="72.5" spans="2:5">
+    <row r="21" ht="75" spans="2:5">
       <c r="B21" s="19" t="s">
         <v>246</v>
       </c>
@@ -8787,7 +8882,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" ht="29" spans="2:5">
+    <row r="22" ht="30" spans="2:5">
       <c r="B22" s="19" t="s">
         <v>249</v>
       </c>
@@ -8796,7 +8891,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" ht="43.5" spans="2:5">
+    <row r="23" ht="45" spans="2:5">
       <c r="B23" s="25" t="s">
         <v>365</v>
       </c>
@@ -8808,7 +8903,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" ht="30" spans="2:5">
       <c r="B24" s="19" t="s">
         <v>368</v>
       </c>
@@ -8822,7 +8917,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="25" ht="58" spans="2:5">
+    <row r="25" ht="60" spans="2:5">
       <c r="B25" s="11" t="s">
         <v>372</v>
       </c>
@@ -8834,7 +8929,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" ht="29" spans="2:5">
+    <row r="26" ht="30" spans="2:5">
       <c r="B26" s="11" t="s">
         <v>374</v>
       </c>
@@ -8896,14 +8991,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="22.2818181818182" customWidth="1"/>
+    <col min="1" max="1" width="22.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="70.2818181818182" customWidth="1"/>
-    <col min="4" max="4" width="47.1454545454545" customWidth="1"/>
-    <col min="5" max="5" width="49.5727272727273" customWidth="1"/>
-    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
+    <col min="3" max="3" width="70.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="47.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="49.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8923,7 +9018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" ht="29" spans="1:5">
+    <row r="2" ht="30" spans="1:5">
       <c r="A2" s="22" t="s">
         <v>379</v>
       </c>
@@ -8963,7 +9058,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" ht="29" spans="2:5">
+    <row r="6" ht="30" spans="2:5">
       <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
@@ -8973,7 +9068,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" ht="145" spans="2:5">
+    <row r="7" ht="150" spans="2:5">
       <c r="B7" s="18" t="s">
         <v>179</v>
       </c>
@@ -9029,7 +9124,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" ht="29" spans="2:5">
+    <row r="12" ht="30" spans="2:5">
       <c r="B12" s="11" t="s">
         <v>357</v>
       </c>
@@ -9041,7 +9136,7 @@
       </c>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" ht="29" spans="2:5">
+    <row r="13" ht="30" spans="2:5">
       <c r="B13" s="11" t="s">
         <v>361</v>
       </c>
@@ -9061,7 +9156,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" ht="43.5" spans="2:5">
+    <row r="15" ht="45" spans="2:5">
       <c r="B15" s="18" t="s">
         <v>246</v>
       </c>
@@ -9082,7 +9177,7 @@
       </c>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" ht="29" spans="2:5">
+    <row r="17" ht="30" spans="2:5">
       <c r="B17" t="s">
         <v>368</v>
       </c>
@@ -9096,7 +9191,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" spans="2:5">
+    <row r="18" customHeight="1" spans="2:5">
       <c r="B18" s="11" t="s">
         <v>170</v>
       </c>
@@ -9138,14 +9233,14 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.14545454545454" customWidth="1"/>
-    <col min="2" max="2" width="23.1454545454545" customWidth="1"/>
-    <col min="3" max="3" width="34.2818181818182" customWidth="1"/>
-    <col min="4" max="4" width="25.1454545454545" customWidth="1"/>
-    <col min="5" max="5" width="33.4272727272727" customWidth="1"/>
-    <col min="6" max="6" width="9.14545454545454" customWidth="1"/>
+    <col min="1" max="1" width="9.14285714285714" customWidth="1"/>
+    <col min="2" max="2" width="23.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="34.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="25.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="33.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9201,7 +9296,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" ht="29" spans="2:5">
+    <row r="6" ht="45" spans="2:5">
       <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
@@ -9223,7 +9318,7 @@
       </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" ht="159.5" spans="2:5">
+    <row r="8" ht="165" spans="2:5">
       <c r="B8" s="18" t="s">
         <v>349</v>
       </c>
@@ -9259,7 +9354,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="12" ht="87" spans="2:4">
+    <row r="12" ht="90" spans="2:4">
       <c r="B12" s="18" t="s">
         <v>246</v>
       </c>
@@ -9270,7 +9365,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" ht="29" spans="2:3">
+    <row r="13" ht="45" spans="2:3">
       <c r="B13" s="18" t="s">
         <v>249</v>
       </c>
@@ -9278,7 +9373,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" ht="72.5" spans="2:4">
+    <row r="14" ht="75" spans="2:4">
       <c r="B14" s="18" t="s">
         <v>365</v>
       </c>
@@ -9289,7 +9384,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="15" ht="87" spans="2:4">
+    <row r="15" ht="90" spans="2:4">
       <c r="B15" t="s">
         <v>406</v>
       </c>
@@ -9308,7 +9403,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" spans="2:4">
+    <row r="17" customHeight="1" spans="2:4">
       <c r="B17" s="11" t="s">
         <v>170</v>
       </c>
@@ -9319,7 +9414,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="18" ht="29" spans="2:4">
+    <row r="18" ht="30" spans="2:4">
       <c r="B18" s="11" t="s">
         <v>173</v>
       </c>

</xml_diff>